<commit_message>
HSBC Referral template (not yet add templates for transaction fields)
</commit_message>
<xml_diff>
--- a/Raw Input Data/Tool_Input_Excel_v4 - Batch 5_v1 (20250619).xlsx
+++ b/Raw Input Data/Tool_Input_Excel_v4 - Batch 5_v1 (20250619).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A8AB57-42F8-488B-B9CA-A2B4B4F928CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5273A49B-FC7A-4C1A-AF37-D6C986A3C4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" tabRatio="706" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" tabRatio="706" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADCC_General" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="ADCC_Txn_Details" sheetId="5" r:id="rId3"/>
     <sheet name="Cross_Border" sheetId="11" r:id="rId4"/>
     <sheet name="CrossBorder_Bene_Details " sheetId="12" r:id="rId5"/>
-    <sheet name="Police_Letter" sheetId="6" r:id="rId6"/>
-    <sheet name="Police_Letter_Suspected_Nature" sheetId="7" r:id="rId7"/>
-    <sheet name="Police_Letter_Txn_Details" sheetId="9" r:id="rId8"/>
-    <sheet name="Police_Letter_Type_Of_Deception" sheetId="8" r:id="rId9"/>
-    <sheet name="CrossBorder_Txn_Details" sheetId="13" r:id="rId10"/>
+    <sheet name="CrossBorder_Txn_Details" sheetId="13" r:id="rId6"/>
+    <sheet name="Police_Letter" sheetId="6" r:id="rId7"/>
+    <sheet name="Police_Letter_Suspected_Nature" sheetId="7" r:id="rId8"/>
+    <sheet name="Police_Letter_Txn_Details" sheetId="9" r:id="rId9"/>
+    <sheet name="Police_Letter_Type_Of_Deception" sheetId="8" r:id="rId10"/>
     <sheet name="Search_Warrant" sheetId="2" r:id="rId11"/>
     <sheet name="UAR" sheetId="10" r:id="rId12"/>
     <sheet name="UAR_Involved_Parties" sheetId="14" r:id="rId13"/>
@@ -37,10 +37,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">UAR!$A$1:$AR$16</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2595,7 +2606,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2654,6 +2665,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2663,7 +2675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3159,13 +3171,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="33"/>
+      <c r="C1" s="34"/>
       <c r="D1" t="s">
         <v>99</v>
       </c>
@@ -3174,7 +3186,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
@@ -3664,26 +3676,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>114</v>
       </c>
@@ -3694,22 +3706,25 @@
         <v>291</v>
       </c>
       <c r="D1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="E1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3719,623 +3734,436 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>311</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>351</v>
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>313</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>315</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>351</v>
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>313</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>315</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F5" t="s">
-        <v>313</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>23</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>483</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="B10">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>315</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F6" t="s">
-        <v>313</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>315</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F7" t="s">
-        <v>313</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>315</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F8" t="s">
-        <v>313</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>311</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F9">
-        <v>122222221</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>311</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="F10">
-        <v>122222221</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
       <c r="C11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>311</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="F11">
-        <v>122222221</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>46</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
-        <v>315</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="F12" t="s">
-        <v>313</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>46</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>439</v>
-      </c>
       <c r="D13" t="s">
-        <v>315</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>458</v>
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>313</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>25</v>
-      </c>
-      <c r="B14" s="1">
+        <v>47</v>
+      </c>
+      <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>315</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1">
+        <v>4</v>
+      </c>
+      <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>311</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>455</v>
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>311</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>455</v>
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>315</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>27</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>315</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>27</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>315</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>27</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>315</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>47</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>311</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="F22" t="s">
-        <v>313</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>606</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="F23">
-        <v>122222221</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="F24">
-        <v>122222221</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
-        <v>311</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>311</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>455</v>
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>483</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -4344,6 +4172,18 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000INTERNAL</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000000000000}">
+          <x14:formula1>
+            <xm:f>COMMON!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:H2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4388,45 +4228,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="33" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
@@ -5700,7 +5540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AR43"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="T34" sqref="T34"/>
@@ -5752,63 +5592,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33" t="s">
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
+      <c r="AO1" s="34"/>
+      <c r="AP1" s="34"/>
+      <c r="AQ1" s="34"/>
+      <c r="AR1" s="34"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
@@ -8262,7 +8102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:X187"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
@@ -10713,7 +10553,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10727,21 +10567,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
@@ -11119,8 +10959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11570,7 +11410,7 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="36" t="s">
         <v>542</v>
       </c>
       <c r="E16" t="s">
@@ -11947,6 +11787,692 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F5" t="s">
+        <v>313</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>315</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F6" t="s">
+        <v>313</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" t="s">
+        <v>313</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F8" t="s">
+        <v>313</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F9">
+        <v>122222221</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="F10">
+        <v>122222221</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>311</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="F11">
+        <v>122222221</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>315</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="F12" t="s">
+        <v>313</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="D13" t="s">
+        <v>315</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F13" t="s">
+        <v>313</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>311</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>311</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>315</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>315</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>311</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F22" t="s">
+        <v>313</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F23">
+        <v>122222221</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F24">
+        <v>122222221</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>311</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>311</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000INTERNAL</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z34"/>
   <sheetViews>
@@ -11983,41 +12509,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
@@ -13375,7 +13901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -13778,11 +14304,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -14049,7 +14575,7 @@
       <c r="D13" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="32">
         <v>10000</v>
       </c>
       <c r="F13" t="s">
@@ -14225,539 +14751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:I18"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>290</v>
-      </c>
-      <c r="C1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>31</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>28</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>483</v>
-      </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>28</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>28</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>46</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>47</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>47</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" t="s">
-        <v>483</v>
-      </c>
-      <c r="F18" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000INTERNAL</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000000000000}">
-          <x14:formula1>
-            <xm:f>COMMON!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:H2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A8F4FDE63F23240996C0B5ED71CAB02" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61b2ee7a38442529347de99e33b69841">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc14db02-3d39-436b-9056-63d1dbe054e8" xmlns:ns3="5ed3fcfa-dd51-4f96-90c6-6669337cd654" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="405649729e347460199c909c216f19f3" ns2:_="" ns3:_="">
     <xsd:import namespace="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
@@ -14952,26 +14946,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37988534-FF4F-46F8-84AB-48CC87B76A1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
-    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C7C7C0F-FE5C-4F1B-9A47-80D1E428EC66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4BFD85F-A260-4B68-8370-89136DBE3129}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14988,4 +14983,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C7C7C0F-FE5C-4F1B-9A47-80D1E428EC66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37988534-FF4F-46F8-84AB-48CC87B76A1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
+    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>